<commit_message>
Charts, dropdown menu, styling, notes, and python scripts added
</commit_message>
<xml_diff>
--- a/data/Employed 2015-2021 by Quarter Ukraine.xlsx
+++ b/data/Employed 2015-2021 by Quarter Ukraine.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156393AA-E5B9-4480-B4B4-5D653FD11DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09729386-89C3-4E92-973B-132F74576E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1794,8 +1794,8 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E94" sqref="E94"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>

</xml_diff>